<commit_message>
Updated Table of Contents
</commit_message>
<xml_diff>
--- a/Table_of_Contents.xlsx
+++ b/Table_of_Contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notes\Code Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D713C9A-EC02-4D85-9B80-FC1729C54297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAE2D8F-D3F1-434D-99AD-1ADAA75F4FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>Index</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Closest Neighbhour in BST</t>
+  </si>
+  <si>
+    <t>Pairs Violating BST property</t>
   </si>
 </sst>
 </file>
@@ -470,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E24"/>
+  <dimension ref="A2:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -811,6 +814,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>